<commit_message>
Update PU Learning Usage Principles and refactor dPULearn.fit, dPULearn.eval
</commit_message>
<xml_diff>
--- a/aaanalysis/_data/benchmarks/Overview.xlsx
+++ b/aaanalysis/_data/benchmarks/Overview.xlsx
@@ -214,7 +214,7 @@
     <t xml:space="preserve">Prediction of gamma-secretase substrates</t>
   </si>
   <si>
-    <t xml:space="preserve">Breimann et al, 2023c</t>
+    <t xml:space="preserve">Breimann et al, 2024c</t>
   </si>
   <si>
     <t xml:space="preserve">1 (substrate), 0 (non-substrate)</t>
@@ -350,15 +350,15 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.28"/>

</xml_diff>

<commit_message>
Add Avg length to overview
</commit_message>
<xml_diff>
--- a/aaanalysis/_data/benchmarks/Overview.xlsx
+++ b/aaanalysis/_data/benchmarks/Overview.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t xml:space="preserve">Level</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve"># Sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg length</t>
   </si>
   <si>
     <t xml:space="preserve"># Amino acids</t>
@@ -233,8 +236,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -317,7 +321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -327,6 +331,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -347,27 +355,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="66.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="53.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="66.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="53.21"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -398,28 +407,32 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
+        <f aca="false">E2/C2</f>
+        <v>796.587982832618</v>
+      </c>
+      <c r="E2" s="2" t="n">
         <v>185605</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="F2" s="2" t="n">
         <v>705</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="G2" s="2" t="n">
         <v>184900</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>13</v>
@@ -430,60 +443,68 @@
       <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>71</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
+        <f aca="false">E3/C3</f>
+        <v>831.028169014085</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>59003</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="F3" s="2" t="n">
         <v>163</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="G3" s="2" t="n">
         <v>58840</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>342</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
+        <f aca="false">E4/C4</f>
+        <v>345.754385964912</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>118248</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="F4" s="2" t="n">
         <v>35469</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="G4" s="2" t="n">
         <v>82779</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>20</v>
@@ -494,60 +515,68 @@
       <c r="J4" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>573</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
+        <f aca="false">E5/C5</f>
+        <v>546.205933682374</v>
+      </c>
+      <c r="E5" s="2" t="n">
         <v>312976</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="F5" s="2" t="n">
         <v>2416</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="G5" s="2" t="n">
         <v>310560</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="3" t="n">
+        <f aca="false">E6/C6</f>
+        <v>248.873303167421</v>
+      </c>
+      <c r="E6" s="2" t="n">
         <v>55001</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="F6" s="2" t="n">
         <v>6492</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="G6" s="2" t="n">
         <v>48509</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>27</v>
@@ -558,60 +587,68 @@
       <c r="J6" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K6" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>233</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="3" t="n">
+        <f aca="false">E7/C7</f>
+        <v>796.587982832618</v>
+      </c>
+      <c r="E7" s="2" t="n">
         <v>185605</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="F7" s="2" t="n">
         <v>101082</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="G7" s="2" t="n">
         <v>84523</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="H7" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>1414</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="3" t="n">
+        <f aca="false">E8/C8</f>
+        <v>6</v>
+      </c>
+      <c r="E8" s="2" t="n">
         <v>8484</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="F8" s="2" t="n">
         <v>511</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="G8" s="2" t="n">
         <v>903</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>36</v>
@@ -622,28 +659,32 @@
       <c r="J8" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>7935</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="3" t="n">
+        <f aca="false">E9/C9</f>
+        <v>424.030245746692</v>
+      </c>
+      <c r="E9" s="2" t="n">
         <v>3364680</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="F9" s="2" t="n">
         <v>3864</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="G9" s="2" t="n">
         <v>4071</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>41</v>
@@ -654,28 +695,32 @@
       <c r="J9" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2547</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="3" t="n">
+        <f aca="false">E10/C10</f>
+        <v>241.252453867295</v>
+      </c>
+      <c r="E10" s="2" t="n">
         <v>614470</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="F10" s="2" t="n">
         <v>897</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="G10" s="2" t="n">
         <v>1650</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>46</v>
@@ -686,28 +731,32 @@
       <c r="J10" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K10" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>1835</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="3" t="n">
+        <f aca="false">E11/C11</f>
+        <v>399.126975476839</v>
+      </c>
+      <c r="E11" s="2" t="n">
         <v>732398</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="F11" s="2" t="n">
         <v>1045</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="G11" s="2" t="n">
         <v>790</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>51</v>
@@ -715,28 +764,32 @@
       <c r="J11" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>17408</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="3" t="n">
+        <f aca="false">E12/C12</f>
+        <v>254.611040900735</v>
+      </c>
+      <c r="E12" s="2" t="n">
         <v>4432269</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>8704</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>8704</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>54</v>
+      <c r="G12" s="2" t="n">
+        <v>8704</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>55</v>
@@ -747,95 +800,110 @@
       <c r="J12" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K12" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>6668</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="3" t="n">
+        <f aca="false">E13/C13</f>
+        <v>400.673365326935</v>
+      </c>
+      <c r="E13" s="2" t="n">
         <v>2671690</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="F13" s="2" t="n">
         <v>2574</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="G13" s="2" t="n">
         <v>4094</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="H13" s="2" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="3" t="n">
+        <f aca="false">E14/C14</f>
+        <v>737.809523809524</v>
+      </c>
+      <c r="E14" s="0" t="n">
         <v>92964</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>63</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="2" t="s">
         <v>64</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>65</v>
       </c>
+      <c r="K14" s="0" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>694</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="3" t="n">
+        <f aca="false">E15/C15</f>
+        <v>712.57060518732</v>
+      </c>
+      <c r="E15" s="0" t="n">
         <v>494524</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="F15" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="G15" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>64</v>
+      <c r="I15" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>